<commit_message>
aligning text in tech-bar
</commit_message>
<xml_diff>
--- a/TZ-portfolio.xlsx
+++ b/TZ-portfolio.xlsx
@@ -198,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -214,6 +214,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -517,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F7" sqref="A7:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,22 +594,22 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="8">
         <v>15</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="8">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -679,43 +683,51 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>5</v>
       </c>
@@ -723,13 +735,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>6</v>
       </c>
@@ -737,13 +749,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>7</v>
       </c>
@@ -751,7 +763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
modal gallery for laptop l
</commit_message>
<xml_diff>
--- a/TZ-portfolio.xlsx
+++ b/TZ-portfolio.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>№</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t xml:space="preserve">переделать модальное окно </t>
-  </si>
-  <si>
-    <t>зум</t>
   </si>
 </sst>
 </file>
@@ -522,7 +519,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,15 +597,9 @@
       <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="8">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>